<commit_message>
Partie 1 et 2 ajoutées
</commit_message>
<xml_diff>
--- a/partie2-data.xlsx
+++ b/partie2-data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benji/dev/cpp/projet-c-L2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1C3BF71-B100-C146-8C20-A5FC23B7DD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52F95C6-D98E-424A-8E1F-CC403218B85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{B8569E09-0510-6446-B187-03F3496254A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5C6870-F497-9B4A-99D3-9ACFE2800519}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>